<commit_message>
Update: Update, delete, edit
</commit_message>
<xml_diff>
--- a/Salary.xlsx
+++ b/Salary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Freelance\Freelance_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CACCC8-4381-4194-A12F-5902DE27F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8786859A-A527-40C3-A226-D49CC83FBFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="44">
   <si>
     <t>+ Viết script automation</t>
   </si>
@@ -225,6 +225,17 @@
         -&gt; Thêm check valid, nếu invalid thì vẫn cho add thêm code. (Done)
         -&gt; Merge vô login để thêm 1 chỗ nhập ver code 
         -&gt; Check code có trên DB không, valid k? </t>
+  </si>
+  <si>
+    <t>23. Hiển thị list data trên admin 
+        -&gt; Hiển thị list code (Done)
+        -&gt; Có thể idit (offer a Hải k edit status), xóa -&gt; xóa thì fix lại cái id trong database (50%)
+        -&gt; Tự động update list (Done)
+        -&gt; Có thể filter (Done)
+21. Thêm key xác thực, đã xài cho TK nào, nếu thành công mới set key thành đã xài (100%, đã xong gen code &lt;=50 valid code)</t>
+  </si>
+  <si>
+    <t>-&gt; Xóa đồng loạt 1 mảng code (Done)</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAE7A80-E863-4FF9-B8A8-0AAA7CBAA458}">
   <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2164,26 +2175,26 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>44759</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>22</v>
+      <c r="C21" s="5">
+        <v>3</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>44760</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>22</v>
+      <c r="C22" s="5">
+        <v>3</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -2335,11 +2346,11 @@
       </c>
       <c r="C36" s="19">
         <f>SUM(C5:C35)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D36" s="21">
         <f>C36*D2*10</f>
-        <v>2124450</v>
+        <v>3540750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: 26, 29, 30
</commit_message>
<xml_diff>
--- a/Salary.xlsx
+++ b/Salary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Freelance\Freelance_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15519D09-77D7-4E29-B8E5-3BAEE957CB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E69D17B-578C-4CC0-895C-63993065B89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="45">
   <si>
     <t>+ Viết script automation</t>
   </si>
@@ -240,6 +240,9 @@
         -&gt; Tự động update list (Done)
         -&gt; Có thể filter (Done)
         -&gt; Xóa đồng loạt 1 mảng code (Done)</t>
+  </si>
+  <si>
+    <t>29. Khi KH đã join thành công, code sẽ đổi thành 'used' và admin không thể sửa status lại, co thể xóa (Done)</t>
   </si>
 </sst>
 </file>
@@ -1976,7 +1979,7 @@
   <dimension ref="B2:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2201,15 +2204,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>44761</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>22</v>
+      <c r="C23" s="5">
+        <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -2350,11 +2353,11 @@
       </c>
       <c r="C36" s="19">
         <f>SUM(C5:C35)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="21">
         <f>C36*D2*10</f>
-        <v>3540750</v>
+        <v>3776800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>